<commit_message>
streamlit app created through uploading audiofile
</commit_message>
<xml_diff>
--- a/Audio_Transcription.xlsx
+++ b/Audio_Transcription.xlsx
@@ -1,63 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>file_name</t>
-  </si>
-  <si>
-    <t>transcribe</t>
-  </si>
-  <si>
-    <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
-  </si>
-  <si>
-    <t>c0fec98f-91de-4349-b21d-25dc05f55eaf_0_r.wav</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> � pivot यlav यदकतिम वोए वोडूथ नहम्यताomp यदकगं सार नह में सय overboard एक य मैंनगके -"3 Insife". ग ग ग गौफle time , 47-24 month ke sa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Yes, yes. In English, okay, final. I'm actually a dark skyward dancer, Hotsolampir, an abomba 27th audio aware of it now. Yes. It was told by him by his teacher. Yes, but so congratulations from that he's been qualified for the next level, National quarter finals. Okay. Which will be on January 3rd, Visma. January 3rd. Yes, yes. January 3rd week. Third week. Okay. Yes, yes. So January 3rd week. Have you received the report card and certificate? Regarding your change, all of you. Is it being needed? One second, ma'am. So one second, I'll let you. Yeah, ma'am. So ma'am, they have shared through the mail ma'am. Have you checked it? I think I have checked it. Yes, ma'am. One second. This will be your mail ID. Ma'am, go L3D28 at the rate of email.com. Yes. Yes, ma'am. Yes, ma'am. Actually, we have shared now, ma'am. Not a problem. I'll be sharing through your whatsapp number also after this call. Okay. Some how was the exam and actual how was the experience of the exam? Actually, he did it himself only. And later we had a discussion. He said that some of the sums like this took time to solve. Otherwise, he was okay. Yes, ma'am. So ma'am, actually, I'll be transferring to the academic counselor. So he will be explaining you clearly now. One second. Okay. Oh no. Oh, what? So, what's the last year? Yes, ma'am. What's the academic counselor? Ranji. Yes. I'll talk about this one. Okay. Okay, sir. Ranji. Yes, children. There is an exam in the online. I'm asking about this regarding the idea. Ranji, what's the lump here? Yes. Yes, ma'am. What's the number? It's 37th of the number. Ranji. So, I know. In case details are available on the mail. I mean, the score card and certificate. I have seen. Okay. So, first of all, I will tell you the congratulations. That's going to be the last one. I have a final round. Yes. I was talking to Arlea. You said quarter final. Sorry. The person who was talking to me earlier. He said that quarter final. Yes. I'm sorry. The person who was talking to me earlier. He said that quarter final. He said that quarter final. Yes. No, ma'am. I'm sorry for incriminating. The organization is new. So, the final round of the child. The number of the child is 2. The first one is the pre-lens date. The final round of the child. Yes. The pre-lens date. The final round of the child. This is February 2nd week. I will bring you back to the next exam. February 2nd week. Yes. So, before one. January 3rd week. Sorry, ma'am. Nothing. You want to be in the field. Yes. So, after two months, I will bring you back to the next exam. It will be the same on the next exam. But, I will bring you back to the next exam. Okay. Pattern will be same or more. Question. Yes. Yes, ma'am. This is a little bit changes. This is completely national wide exams. So, regarding this. Okay. Now, what is the call? Yes. Before the examination, some children will provide a training session. For two months. Okay. Yes. This is also the same. You will be in the online Google Meet. Children will conduct a program. Yes. Yes. It is a HVDS, Higher, Order, Thinking, Skills. Okay. What? Right. Yes. So, ma'am, this is the class structure. It will be weekly twice. And complete. In two months, you will have 16 classes covered. Before examinations. Okay. So, the online structure, ma'am, this is a very comfortable child. This is just weekly class. You can join them in the weekend. And, we can do it. The timing slots are available in our class. Morning, dinner, cup to seven, we will have a time available. The class duration of the day, ma'am, is one level. Forty-five minutes to one level, the class duration is the same. You can also refer them to evening slots. Ma'am, we have a time available for four to five, five to six and six to seven. Okay. Yes. You will have two months of classes. And the best thing is, ma'am, before the classes start, we will conduct a level mapping test. So, we will have more clarity. We need more guidance in which. Ma'am, any child is at an understanding level. Ma'am, there is a mathematics. So, based on the number of the level mapping test, after that, after their classes, Ma'am. Yes. Okay. This is a complete two-minute course. Yes. After that, if you will be interested in the programs, you can continue for other module. Okay. Yes. So, this module will be chargeable, because all the materials in this, all the works will be used. They will provide our teachers. And on and on, it means that you will not be able to get more. Ma'am, only four to six children, we will prepare a batch. Ma'am, they will provide a certified personal teacher. Yes. The children will be comfortable with each other. Okay. Yes. Ma'am, you will go to the weekend, you will go to the weekend. We can stay in the weekend. Yes. Yes. Ma'am, the parents will be able to prepare the weekend. You have to have some time. Yes. If we can stay in the weekend, then it is not an issue. It is free now. Otherwise, we can have some games. Okay. We have lots of things to do. Yes. Ma'am, you are doing a time slot and we have a phone in the weekdays. Yes. We will connect all the classes today. Okay. Ma'am, you will start your classes from Monday. You will start your training formalities, you will have to mail to Ma'am or your WhatsApp report. Yes. It is a mail. First of all, it is a thing that we have got here. Yes sir. This is the free structure. We will charge it basically. It is 5000 years. But it is 5000 years. Yes. It will be GST. But it is a selection of the past dawn in the Olympic. So this is already eligible for scholarship. So we will charge it more. It is basically, we want to pay it. For two months of the complete class, it will be Ma'am 2000, 600 rupees. Okay. For two months of the complete class, plus the work sheets of the Jubis, we will provide the teachers of the children. Yes. It will be in the PDF form. Yes. I am so sorry Ma'am. What are you saying? We will provide the PDF. We will provide the sheets of the work sheets. Yes. Ma'am, we will provide the children in the online. The students of the Olympic Games, they will design the syllabus and provide the students of the level. Okay. Yes. I will confirm your main course. This is the G.O.Y.A.L.T.R.I. T.I.28 at G.M.L.. Right? Right. Yes. So you have to send all the details right now. Which one of you have made? It is weekly twice. It is weekly. It is weekly. Actually, the action going to school when he will come back. I will do it later. So, I will do it later. Otherwise, there is no problem in the weekly. In the evening, I will like 6 to 7. I will do it later. If we do it, I will be able to discuss it with my dad. Sure. Ma'am, please discuss it. Okay. I will send all the details on your mail. Before any 5.3, Ma'am, please give me the internet. Okay? Yes. I will give you the heart's key. The heart's key is not the heart's key. don't be commissive. Right. We will also be able to select this message. Yes, please correct. I am unable to select. Are we able to select? Which is the key? Alright. Otherwise, Oh God! I will ask all right. Anyway, I will comments in this letter with my concrete work. I want to write it out to you. Thank you for the microphone. I will do it there. The grad Armenian coding vaccine is involved in dialogue reversal. You can focus on this program once you get to the registration language. As poetry does not violent in the election. eastern brightness? It provokes especially against anti-opecology Sungish PM from today on. And legs of one minute will be destroyed by war. centered on theny or sub wszystko mi שמ� Ka. The question will be responding to men lolupbeat lightly. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes.</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -72,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -388,38 +420,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>file_name</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>transcribe</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> � pivot यlav यदकतिम वोए वोडूथ नहम्यताomp यदकगं सार नह में सय overboard एक य मैंनगके -"3 Insife". ग ग ग गौफle time , 47-24 month ke sa</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>c0fec98f-91de-4349-b21d-25dc05f55eaf_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Yes, yes. In English, okay, final. I'm actually a dark skyward dancer, Hotsolampir, an abomba 27th audio aware of it now. Yes. It was told by him by his teacher. Yes, but so congratulations from that he's been qualified for the next level, National quarter finals. Okay. Which will be on January 3rd, Visma. January 3rd. Yes, yes. January 3rd week. Third week. Okay. Yes, yes. So January 3rd week. Have you received the report card and certificate? Regarding your change, all of you. Is it being needed? One second, ma'am. So one second, I'll let you. Yeah, ma'am. So ma'am, they have shared through the mail ma'am. Have you checked it? I think I have checked it. Yes, ma'am. One second. This will be your mail ID. Ma'am, go L3D28 at the rate of email.com. Yes. Yes, ma'am. Yes, ma'am. Actually, we have shared now, ma'am. Not a problem. I'll be sharing through your whatsapp number also after this call. Okay. Some how was the exam and actual how was the experience of the exam? Actually, he did it himself only. And later we had a discussion. He said that some of the sums like this took time to solve. Otherwise, he was okay. Yes, ma'am. So ma'am, actually, I'll be transferring to the academic counselor. So he will be explaining you clearly now. One second. Okay. Oh no. Oh, what? So, what's the last year? Yes, ma'am. What's the academic counselor? Ranji. Yes. I'll talk about this one. Okay. Okay, sir. Ranji. Yes, children. There is an exam in the online. I'm asking about this regarding the idea. Ranji, what's the lump here? Yes. Yes, ma'am. What's the number? It's 37th of the number. Ranji. So, I know. In case details are available on the mail. I mean, the score card and certificate. I have seen. Okay. So, first of all, I will tell you the congratulations. That's going to be the last one. I have a final round. Yes. I was talking to Arlea. You said quarter final. Sorry. The person who was talking to me earlier. He said that quarter final. Yes. I'm sorry. The person who was talking to me earlier. He said that quarter final. He said that quarter final. Yes. No, ma'am. I'm sorry for incriminating. The organization is new. So, the final round of the child. The number of the child is 2. The first one is the pre-lens date. The final round of the child. Yes. The pre-lens date. The final round of the child. This is February 2nd week. I will bring you back to the next exam. February 2nd week. Yes. So, before one. January 3rd week. Sorry, ma'am. Nothing. You want to be in the field. Yes. So, after two months, I will bring you back to the next exam. It will be the same on the next exam. But, I will bring you back to the next exam. Okay. Pattern will be same or more. Question. Yes. Yes, ma'am. This is a little bit changes. This is completely national wide exams. So, regarding this. Okay. Now, what is the call? Yes. Before the examination, some children will provide a training session. For two months. Okay. Yes. This is also the same. You will be in the online Google Meet. Children will conduct a program. Yes. Yes. It is a HVDS, Higher, Order, Thinking, Skills. Okay. What? Right. Yes. So, ma'am, this is the class structure. It will be weekly twice. And complete. In two months, you will have 16 classes covered. Before examinations. Okay. So, the online structure, ma'am, this is a very comfortable child. This is just weekly class. You can join them in the weekend. And, we can do it. The timing slots are available in our class. Morning, dinner, cup to seven, we will have a time available. The class duration of the day, ma'am, is one level. Forty-five minutes to one level, the class duration is the same. You can also refer them to evening slots. Ma'am, we have a time available for four to five, five to six and six to seven. Okay. Yes. You will have two months of classes. And the best thing is, ma'am, before the classes start, we will conduct a level mapping test. So, we will have more clarity. We need more guidance in which. Ma'am, any child is at an understanding level. Ma'am, there is a mathematics. So, based on the number of the level mapping test, after that, after their classes, Ma'am. Yes. Okay. This is a complete two-minute course. Yes. After that, if you will be interested in the programs, you can continue for other module. Okay. Yes. So, this module will be chargeable, because all the materials in this, all the works will be used. They will provide our teachers. And on and on, it means that you will not be able to get more. Ma'am, only four to six children, we will prepare a batch. Ma'am, they will provide a certified personal teacher. Yes. The children will be comfortable with each other. Okay. Yes. Ma'am, you will go to the weekend, you will go to the weekend. We can stay in the weekend. Yes. Yes. Ma'am, the parents will be able to prepare the weekend. You have to have some time. Yes. If we can stay in the weekend, then it is not an issue. It is free now. Otherwise, we can have some games. Okay. We have lots of things to do. Yes. Ma'am, you are doing a time slot and we have a phone in the weekdays. Yes. We will connect all the classes today. Okay. Ma'am, you will start your classes from Monday. You will start your training formalities, you will have to mail to Ma'am or your WhatsApp report. Yes. It is a mail. First of all, it is a thing that we have got here. Yes sir. This is the free structure. We will charge it basically. It is 5000 years. But it is 5000 years. Yes. It will be GST. But it is a selection of the past dawn in the Olympic. So this is already eligible for scholarship. So we will charge it more. It is basically, we want to pay it. For two months of the complete class, it will be Ma'am 2000, 600 rupees. Okay. For two months of the complete class, plus the work sheets of the Jubis, we will provide the teachers of the children. Yes. It will be in the PDF form. Yes. I am so sorry Ma'am. What are you saying? We will provide the PDF. We will provide the sheets of the work sheets. Yes. Ma'am, we will provide the children in the online. The students of the Olympic Games, they will design the syllabus and provide the students of the level. Okay. Yes. I will confirm your main course. This is the G.O.Y.A.L.T.R.I. T.I.28 at G.M.L.. Right? Right. Yes. So you have to send all the details right now. Which one of you have made? It is weekly twice. It is weekly. It is weekly. Actually, the action going to school when he will come back. I will do it later. So, I will do it later. Otherwise, there is no problem in the weekly. In the evening, I will like 6 to 7. I will do it later. If we do it, I will be able to discuss it with my dad. Sure. Ma'am, please discuss it. Okay. I will send all the details on your mail. Before any 5.3, Ma'am, please give me the internet. Okay? Yes. I will give you the heart's key. The heart's key is not the heart's key. don't be commissive. Right. We will also be able to select this message. Yes, please correct. I am unable to select. Are we able to select? Which is the key? Alright. Otherwise, Oh God! I will ask all right. Anyway, I will comments in this letter with my concrete work. I want to write it out to you. Thank you for the microphone. I will do it there. The grad Armenian coding vaccine is involved in dialogue reversal. You can focus on this program once you get to the registration language. As poetry does not violent in the election. eastern brightness? It provokes especially against anti-opecology Sungish PM from today on. And legs of one minute will be destroyed by war. centered on theny or sub wszystko mi שמ� Ka. The question will be responding to men lolupbeat lightly. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes. Yes.</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> I like having the people raise my hands and I do frequency connections showing needs My first interpersonal connection with the Hello. Hello. How's our fatta intend, hi, this is really interesting. What's up, Here? My name is Hi. Hi! We're here Hi. Hi guys. Hi. Come back later, you see. The timer Rossia about to turn on the traffic junk to get into delivery. This flight is theрахave an antenna to get up. Uh-huh. Okay. You have already met me already. You are going to be a man. No, no, no, no, no. I told you I'm a man. I was taken. I did not go there. Okay, okay. I'm not going to shoot. You see, I'm sharing. You see, you've got a lot of numbers. You could be like 40 right. Okay, okay. Yeah. So, I think I've got a lot of common little national election you can't prove it. You can't do it. So, that can be on the online list. Yeah. Yeah, that can be on the online list. And you can add in some form. So, you're a smart. So, uh, yeah, I'm interested to call the second round national election. Right? Yeah. So, I choose her here. Uh, the second round, then we need to be in the middle and uh, I'll stand by and then we'll be like, the post-censor layer. It's like, the third round, the example here, preliminary round, post-censor. Okay. So, there's a few things here. Uh, before that, for that, uh, how the question is that coming, how they are going to answer that post-censor like that. And so, two months class elections here will be deployed to the next round. So, that will also online class for the big two days class of here, providing. So, uh, like, the one that you got, uh, big two days. Big two days. So, uh, actually, uh, Monday to Sunday, trainers are available sorry, in big two days you can choose. two months, I choose in, uh, packet as I'm doing this. So, like that, if you are, okay. And also, so, here, I choose for defining issues the class duration thing. And for defining the class, uh, section, uh, so you can take any four defining. So, uh, there are some, uh, I'm not sure if you know that taking, uh, even in back, just like a fight to fight for deep fight back, just a few seconds. Like that. So, basically here, actually, there has been, uh, doing the same thing. So, we all know that, uh, students are by fighting the thing. They are outnumbering. Like, really, we are here. We are helping the students how to understand the questions we told about our working or we told to have them ready. So, how they learn to understand the question on how they can answer it. Like that. Okay. Okay. So, uh, the second question is, uh, having a doubt. So, uh, this, this program is, uh, and complemently, uh, are there some charges in it? Okay, so, uh, the class is based on the YouTube, uh, so, uh, while you are doing that in session routine, you can do a, uh, 25-month-olds, 24-day-in-date human class section. for the piece for the human class, we have two months class section for 22-day-in-date class section. Okay. Okay. So, uh, I will share the answer the decision on the whole, uh, uh, you are going to report this round. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Okay. Any queries on how everything you've played? Um, I think for now, you just send me a little bit of both of it. Okay. Okay. Okay. Okay. Thank you so much. Thank you. I see a big one. I hope you just come later. It's just because two months time already. Okay. So, it will take only two months. It will take four years session only two minutes to take. So, just take it from only two minutes. Okay. So, anyway, I'll share the only answer. So, I just go through that and let me know. Okay. Okay. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>live such to times address you media Word language air For local Okay Sorry The What the visibility losraphic yeah In кан Attendant seni Tool yeah Oh so So basically here before that exam, I think we are giving 200 class collections for the class. The how the questions are coming, how they are going to answer the questions like that and so 200 class collections, we are going to provide the correct answers. So that we want to online class for the BP today's class of the year, providing. So like the Monday, the VK2 days, VK2 days, we get to read, we get to read, we get to read. So actually Monday to Sunday, Friday, Saturday, Wednesday, we get to read, we get to read from Thursday to Wednesday to Friday, Saturday, Saturday. So like that is your okay. And also, so here I see for defining issues the class duration thing and for defining this class duration, they're also like morning 8 of the full evening 8 of the club, sections are there so you can take any full defines. So there also, I'm also taking them to a taking, even in practice, even in practice, like a fight to fight for, fight back to sections. Like that. But basically here actually there are things that are doing good there, I, 11 and also thinking about the things that we all know that the students are by fighting the things that are not the money thing. But actually there here we are, the things that students have to understand the questions, we thought about having already thought to have them ready. So how they understand the question on how they can answer it. Like that, they are teaching the students in class. This is still alive, as the sections are going on. Like guys. Okay, okay. So I'm sorry that was a little bit, I saw it in the house. So this program is, and complimenting or are there some charges in it. I can even say, it's a classic page class or YouTube, so you can do it with a class piece. So while you are doing that, it's just a routine, you can do a page that is there among those two, that's what it's for, the end date, human class section. Okay, complimenting for your comments, and complimenting for your comments, class sections for 2000 pages, the end date, class section. Okay, okay. So I answer the, I answer the decision on the one, so you are going to report cards, practicating on the two, and the program will show on the side of the the, you know, watch the number. So you can get this to the, the decision, like this, and then you have your new, you know, watch the, so the, the decision, you will be active. After, you can just keep going, so you can be going, so, because, you need to fill up some, uh, basic information about that, like, like, I said, which I, which I, which I, did, uh, get like that. So after the decision, you can, uh, the share with the screenshot, and also they go for the, and so I, uh, then the admission from, uh, in the system. But tomorrow, we, uh, tomorrow, you look at the course from admission, do you show you can, do the any, you have to see, if it's, then you want the class section, and, uh, the letter. Okay. Okay. So you have any queries, how you have everything you have to hear? Um, I think for now, you, uh, send me a little bit, uh, go through it. Okay. Okay. Okay. Okay. Okay. So, okay. Thank you, sir. Thank you. I see it before. I hope you just come later. It's just, you know, because two months time, or you need to start the class section. So, I, I, I, I, I'm so, really. Okay. So, if you will take, if you will take only two minutes, uh, it will take four sessions, only two minutes, if you will take, uh, so just, uh, take it from, only two minutes, okay. So anyway, I'll share the only answer. So I just go through that and, uh, let me know. Okay. Okay. Okay. Thank you. Have a nice day. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> So, leave them with me up here now.ünden f Hi. I get me at a job shoot, there you are.UT Start modeling. Disockey floor. Can you be my director or director? Can you mention? Are we going to do it? Going forward?nínu arque m membrna xlioe jabt. I am very happy to see you again. Yes, I am very happy to see you again. Yes, I am very happy to see you again. You have already met me already. You are going to be a man. Yes, I have taken it. I have been using it for a long time. I have been sharing it with you a lot of times. I have been sharing it with you a lot of times. Yes, so I have been sharing it with you a lot of times. Yes, I have been sharing it with you a lot of times. Yes, I have been sharing it with you a lot of times. Yes. Yes, so I have checked here. The second round, we have been using it on the other end. We have checked here, we have checked here. The second round, we have been using it on the other end. So basically, here, before that exam, we are giving 200 class collections for the class. The whole question is coming out there, one door, and the other door is like that. So, 200 class collections, we are going to provide the correct answer. So, that amounts of online class for the BP, 2 days class of the year, providing. So, like a Monday or Monday? Work 2 days or 때 classes, we keep do way out. Yes, we keep do day so. So, we can actually warn the class that a lot of people are mulling to day classes, of most thing we do not teach the class during our classes and didn't. So, like that is if you are okay. And on social here, I teach for defining issues the class duration thing. And for defining the class duration, they're also like morning eight of group, evening eight of group, sections are there. So, you can take any four defines. So, there are some, I'm not taking them that taking evening classes, like a fight or a fight or a fight or a fight or a section. Like that. So, basically here actually there are things that are doing good there, I, Q 11 and also thinking about the things that we are not that are, children are by fighting the things that are not normal things. But actually there here we are, and things that children are too to understand the questions, we thought about a fight or we thought to have a memory. So, how they understand the question on how they can answer it. Like that, they are teaching the children's in class. This is still our life, our sections are going on. Like that. Okay, okay. So, I'm sorry that was a little bit, I saw a little doubt. So, this program is, and complimenting, or are there some charges in it. I can tell you, it's a classic page class, or YouTube, 2000, or 50, a class, YouTube. So, while you are doing that, it's just a routine, you can do page, it's a month, or two, or so, 24, then get to a month class section. Okay, so, I have a little bit of a compliment, and a two month class section, for 2000, you can say, a 20-day class section. Okay, okay. So, I will share the answer that is sitting on the old floor, you are going to report cards, practically, you can also do a month program, or you should also share the, you need a lot of number. So, you can just do the relationship like this. There's a lot of people, you can just do it. So, if you're not doing it, you can do it. You can just do it. So, you can do it. So, because you need to fill up some basic information about that, like, besides, you need to say, you need to get like that. So, after the discussion, you can share with the screen shot, and also, they go for the top of the page, and show IE, then the admission from IE, but tomorrow, you look at the course from admission. You can show it in the empty page, if you pay me one, the class section, and the leg, then. Okay, so, you have any queries? How are you, everything you've created? I think for now, I'll go through it. Okay. Okay, so, thank you, sir. Thank you. I see a big four-fire group of you just come later, and it's just because two months' time, or you need to start the class, and so do it. So, today, I'm so real. But I am okay. So, if you will take, if you will take for your doings, if you will take for a session, or you need two minutes, if you will take. So, just a ticket, or you need to finish it. Okay, so anyway, I insured or you can start. So, I just go through that, and let me know. Okay. Okay, sir, okay, thank you. Have a nice day. Thank you, sir.</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Thank you. Hello. Hello. Hello. Hello. Hello. Hello. You are still amazement to Klimtter се. Pardon you. Yeah. Pardon me. For temperat Hybridd. Well, I am. Bon environment. Welcome to this job. Disklept all this time. Very good. From the time that 11,000 people are participating in our next service. I'm sure it will be alright. Because I'm all I'm going to. Are you aware of what that one said? Yeah. Okay. So actually I want to inform you that I see these parts of the first home victims. And also, the people for this, I can know it upcoming, the real national victims. But I'm not going to get some of those parts. Okay. So, I'm getting a little bit of an amazement regarding my child to work on. I'm so too cute. You can feel it. Yes, it's a really nice. Uh-huh. So, you saw that the work on amazement, the work on that ticket. Uh-huh. Okay. You have already met me already. You are going to. No, no, no, no. I told you I'm in. I already wanted to. I was. Yeah. I'm taking it. I did not work. Okay. Okay. I'm not going to shoot it. You see I'm sharing a bit of a lot of my anxiety. I'm sharing a lot of number of people. You could be like 40, right? Okay. Okay. Yeah. So, I think I've got to come on top of the little national election. You can't really have to do any technical. So, that can work on online next door. Yeah. Uh-huh. Yeah, that can work on online next door. You can have them come from. So, you will swap. So, uh-huh. Yeah, I'm just going to call the second one national election. Right? Oh. Yeah. So, I'll choose her here. Uh-huh. The second one, I can go and really think easily. Uh-huh. I'll stand by. So, I'll be right to death. The constant only up. It's right. So, the third one, I can go and move here. Or more. Uh-huh. I'll be right back. Okay. So, the second one is here. Uh-huh. Before that, I can go and choose. I'll give you two more classes. I'll change for the next. The how the questions are coming. How they are going to answer the questions like that. And so, two months class, that's actually a point to prove it. The correct answer. So, that will also online class for the big two days class of the year. Providing. So, uh-huh. I'm going to run. A big two days. Big two days. Yeah. Big two days. So, if I actually uh- Monday two Sunday, trainers are available. Sorry. In big two days, we can choose. From mostly two months, I choose in a packet. I'm just. So, like that is your. Okay. And also, I hear I choose for the five minutes with the class duration thing. I'm for the five minutes class duration. I'm also like morning eight of the food, evening eight of the club. Um, uh, sections are there. So, you can take any food designs. So, uh, there are some, uh, I'm also taking them to a ticket, uh, evening back. This evening back, it's like a flight to flight for the flight back to sections. Uh, two weeks ago. Like that. But basically here, actually, there has been a time to remove their IQ 11 and also thinking about the ticket. So, we all know that uh, the students are by fighting the thing. They are outnumbering. Like, we hear we are in the students how to understand the questions. We told them by fighting or we told them how to remember it. So, how they understand the question and how they can answer it. Like that, they are teaching the students in class. This is still our life. As sections are going on. Like that. Okay, okay. So, uh, the standard procedure, uh, having a dose. So, uh, this program is uh, uncomplimentary or uh, are there some charges in it? Uh, I can measure, uh, the classes take class only. Two thousand rupees with a class fee. So, uh, while you are doing that, if you're sitting in the end, you can do a paid uh, a paid amount of two thousand rupees for the end date to one class section. Okay. So, I'll give you a piece for two months, please. We are two months class sections for two thousand rupees. The end date class section. Okay. Okay. So, uh, I'll share the, uh, I'll share the session and also, uh, uh, you are going to report a certificate and I want to do a month program. So, I'll share the, uh, you need a lot of number. So, you can just do the session. Like this, it can be a high, you need a lot of number. So, the session in will be active. Uh, after you can just keep going. So, you need to fill up some basic information about that like, uh, size, which I mean, size, uh, paid like that. So, after the session, you can, uh, share with the screenshot and also, date over top, but then so I will, uh, then the admission from I need to. But tomorrow, we, uh, tomorrow, you look at the course from admission. Do you show you can shoot in your basic certificate? Then you want the class section and then, uh, like that. Okay. Okay. So, you have any queries or you have everything you have to? Um, I think for now. You, uh, send me a little bit, uh, go through it. Okay. Okay. Okay. Okay. Okay. Okay. Thank you, sir. Thank you. I see a default period. Just commenter, since that, because tomorrow time, you need to start the class and so, do you? That's a trick today. I'm so real. But I don't know. Okay. So, if you will take, if you will take for lecture minutes, uh, if you will take for a session, or lecture minutes, if you will take, uh, so just, uh, take it. Or lecture minutes? Okay. So anyway, I will share the old details, uh, so I just go through that and, uh, let me know. Okay. Okay. Okay. Thank you. Have a nice day. Thank you. Nice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> gates So very good from the time that the time was particularly better than some of these who said my soul and the are because I know all I make some are you aware of what that wants to do you do actually I want to inform you that I see you fast the fast from the and also you can focus on upcoming level national level of the and the and the and the the and the the the the and and and and and and and either another and yeah and and and that and again and yeah so that have a comment a little last and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and dumb can and but but and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and and</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Elesim Hello Yes Yes So Nice I got me a job with變 sweetness for a little bit on my message emphasis on the cause of gentle from this emotion of death Raf freelancer and okay you are arbe$towning Y counted the better yes a Miss Y a you are you are okay out of by the does up up I use a defining instance to class duration thing. I'm for defining class duration, then also like morning 8 o'clock, evening 8 o'clock sections are there. So you can take any four defineings. So there also, I'm also taking them to a taking, evening 8 o'clock, evening 8 o'clock, like a fight to fight for, detaite by some sections. Ah, Tuesday itself. Like that. So basically here actually, the thing that I do in route there, I do live and also thinking about it. So we all know that, ah, childrens are by fighting the thing, they are not numbering. So actually, we are here, we are helping the childrens how to understand the questions, be told by having a little bit thought to the homeworky. So how they understand the question and how they can handle it. Like that, be a teaching of the childrens in class. This is teaching our life, as sections are going more. Like this. Okay, okay. So, ah, the second question is, ah, having a doubt. So, ah, this program is, ah, and complementing or, ah, are there some charges in it? Ah, here is a, ah, it's a classic big class of YouTube, so you can do it with a class piece. So, ah, while you are doing that, as you are sitting in the end, you can do a big, ah, a few more notes. 2000, 64, then, then, two month class sections. Okay. So, further, please put two month classes. We are two month class sections for 2000 pieces. Then, then, class sections. Okay, okay. So, ah, I will share the, I will share the, the section, and also, ah, ah, you are going to report a practical, and I want to do a month program for all the roles I share, that the, ah, you need to watch a number. So, you can, just do the, the section. So, this, take me high, you need to watch up, so, the section, you need to be active. After, you can, just keep going, you, so it will be going, so, because, ah, you need to fill up some, ah, basic information about, ah, like, ah, site, site, site, uh, date like that. So, after, the section, you can, ah, the share, you can, ah, you can, ah, the share, you can, ah, the screen show. they, they, they, they, they, they, they, they, they, they, they, they, they, you get to, they, you affect the project, they, you affect the project, from the project, from the, of course. Okay. So, tomorrow will be recorded, So, are you, how are you everything Your Playing? Um, um... um, I think for now, um, Um, Um, I think for now, and me as both of us, and we got three, the class, so, I, I'm so, real. But I, okay. So, if you will take, if you will take, or you will, if you will take, or you will, if you will take, so, just, uh, take it from, or you will, if, okay. So, anyway, I'll share the old details, so I just go through that, and, uh, let me know. Okay. Okay. Okay. I'm going to have a next class. Thank you. Thank you. You're welcome.</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Choose A Narrative months market third transportation I actually do not hear me out in the children's house to understand the questions. You don't abide by having or with total of number 80. So how they understand the question on how they can handle it. Like that, they are teaching the children's in-class. This is still alive as such since I was going on. Like this. Okay, okay. So I decided to go to the area, sorry, get out. So this program is uncomplimentary or are there some charges in it. I can tell you that it's a classic, classic, or you two thousand rupees with a class fee. So while you are doing that, if you are just a little tiny, you can do a paid, a few cents more notes. Two thousand rupees for the end of the human class section. Okay, so I will go to the middle of the class section. Yeah, two months class section for two thousand rupees for the end of the class section. Okay, okay. So I will share the answer that is in Android. So you are going to go to the top of the page and you can go to the middle of the program. So you can just do the research. So you can just do the research. So you can just keep going. So you can go in. So some of the people that you need to fill up some basic information about that. Like, like, I would say, you need to pay that. So after the decision, you can just share with the screenshot and also take over the top page. And so I will be done by admission from the end of the page. But tomorrow, you will get the form admission. You can do it in your basic, basic, then you want the class section and fill up the list. Okay. So you have any queries or you have everything you have to. I think for now. You are going to send me a little bit. Okay. Okay. Okay. Okay. Thank you so much. Thank you. I see a before fire. Hopefully you just come later. It's just because two months time already, you need to start the class section. So I took the day. I'm so real. Okay. So it will take only two minutes. It will take for a session only two minutes. It will take. So just a ticket. Only two minutes. Okay. So anyway, I'll share the only cancel. So I just go through that and let me know. Okay. Okay. Okay. Thank you. Have a nice day. Thank you. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> The have he Thank you for your support. Thank you very much.</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>ety Perma Hello, hello, how's everything good off you? good off everybody too, I mean oh, the judge put their in the My name is much much I'm calling from the community and my name is much much more important from the club that we get disclipses of the that regarding some things I'm looking at particularly better than some of the spurs so in the area all I make are you aware of what that yeah okay so actually I want to inform you that I see you in part of the first round exam and also you can focus I can know it's upcoming that national exam most important okay so you're getting the main regarding the charity to board the exam okay you get the key yes it is 10 minutes so you saw that the board can be that okay you have already been already you are going not not not not not not not not not or I a I can I I I I I I I I I or I I okay take Questions Providing Hi But actually I actually I for Beveling Tri— случае r r me what I think we're going to have a memory. So how they will understand the question on how they can answer it. Like that, they are teaching the students in class. If you steal our life, our sections are going wrong. Like this. Okay, okay. So, I'm sorry, I'm not saying it, I'm sorry, I need a dose. So this program is when complimenting or are there some charges in it. I think there are classes, they are going to be 2000 rupees a class fee. So while you are doing that, you can do a fee of $2.64 for the end of the human class section. Okay, so that is the piece for the human class. And the human class section for $2.64 for the end of the class section. Okay, okay. So I will share the answer for the session and also you are going to have to pick it up on the human program. So I said that the human class of number. So you can just do the research in class. It's a thing we have in your work. So the research in human will be active. After you can just keep going. So it will be going. So something because you need to fill up some basic information about that. So I like to say, which I made, I did a bit like that. So after the decision, you can share with us. And also they go for the first and so I need them the admission from I need to send. But tomorrow, tomorrow you look at the form admission. You can do it in your basic, basic, then you want the class section and the lecture. Okay, so you have any queries or you have everything you have to get? I think for now. You are going to send me a little bit more to it. Okay. Okay. Okay. So thank you so much. Thank you. I see it before. I hope you just come later. It's just because two months time or you need to start the class. So I will just treat today. I'm so real. But I got it. Okay. So it will take for a little bit. It will take for a session or a little bit. So just a little bit. Okay. So anyway, I'll share the old details. So I just go through that and let me know. Okay. Okay. Thank you.</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added recorded audio option
</commit_message>
<xml_diff>
--- a/Audio_Transcription.xlsx
+++ b/Audio_Transcription.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -577,6 +577,410 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>c0fec98f-91de-4349-b21d-25dc05f55eaf_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two Two One Two Two Two Two Two Two Two Two Two Two Two Three Two Two Two Three Three Two Three Two Two Two Two Three Two Two Three Two Three Three Three Three Three Two Three Two Two Two Two Two Two Three Two Three Two Three Three Three Three Four Four Three Four Three Three Three Four Three Three Three Four Three Four Three Four Three Three Three Three Two Three Four Three Four Three Four Three Two Three Four Three Four Four Three Four Three Four Three Four Three Four Three Four Three Three Three Three Four Three Four Three Four Three Four Three Four Three Four Three Four Three Three Three Four Three Four Three Four Three Four Three Four Three Four Three Three Three Three Three Four Three Four Three Four Three Four Three Four Four Four Four Four Four Three Four Four Four Four Four Four Four Four</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>c0fec98f-91de-4349-b21d-25dc05f55eaf_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Trump Yes, one second. Now this can be your main lady. Nam goyel, who people and people and people that they don't give in, don't go. Yeah. Yes, I certainly have shared long ago a lot of problems I was sharing two new WhatsApp members on so after this phone. Okay, then, some homes are examined and some homes are examined and some homes are examined. Actually, we did it here in the direction of the phone. And later, we had a discussion. He said that some of the some like two times also a little bit of a little bit. Yes, so, now, I'm going to be transferring to the Academy Council. I'm so even big, I'm going to be doing this. One second. Okay. Okay, so, I'm going to be a little bit. Okay. Okay. Okay. Okay. Okay. Okay. Okay. So, Uh, okay, okay. This is the okay. So, first of all, I don't know what that is. Uh, that's good. I will not beg me for the next time I have fine. I'm going to give a round. Um, there are five of us talking to one of the four three of us talking to one of the four three of us. Sorry. Um, you can talk to one of the three. Um, um Meg. I'm so sorry for you. Um, um, um, um, um, um, um, um, um, um, um, um, um, um, um, um, um, we think Next. Then, uh, Yeah,irdi Coverer not well Yes. We review the Mic Band day Sp now but in Islam a selection of I want On a crescent near in completely completely totallygend Butflanzencin bad bad SUBSCRIBE Pretty good the youtube in the the in fifty 갔 intimidated a wing weighs like</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> So many evidence, oh be sarcastic Please E posição water So Hello Hello Ook me Good uh feature was ok so actually I want to inform you then I definetely motor to fast phone like seams and the Nakeste ok ok ah so you thought that the port car and the port car and that to get ah ok you have already met already you are not not my choice be a man I already want to be a man I will take it I did not hope ok I will take it ok my oh and and quickly how you</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\AppData\Local\Temp\tmpz34v50gk.wav</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\AppData\Local\Temp\tmp1pvwug4p.wav</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\AppData\Local\Temp\tmpo1liezjy.wav</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\AppData\Local\Temp\tmpxaf3i36f.wav</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\AppData\Local\Temp\tmpw78d2un_.wav</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> suppose i will use ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\AppData\Local\Temp\tmpc3d0gpj_.wav</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 1.5% 1.5% 1.5% 1.5%</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\AppData\Local\Temp\tmps2_09x7h.wav</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\AppData\Local\Temp\tmp1x_tegd_.wav</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> adherence</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\MY WORK\openai_voice_analytics\audio.wav</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Rh горje Chirg Rh gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\MY WORK\openai_voice_analytics\audio.wav</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>簡爽 prof станов</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Pleasegras Pleasegras Hello oh, hello Hello This all Well, thank The I Jason给我 the mail immediately more Yeah So Support I000 Yes Congratulations Yes youd , , , , . , , , , , , , , , ma , important okay okay okay thank you thank you I see a before fire for you just come later it's just not because too much time or you need to start the class and so good luck I took today I'm so good but I got okay so if you will take if you will take for a little bit to make a for a session or little minutes you will take so just take it for a little minutes with okay so anyway I will share the old details so I just go through that and let me know okay okay okay thank you have a nice day</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> heavens That's true Red Does the bulldog have a message in it to get a Aha You already want me to place you with NO I'm a member Xiao Lan, check there No other long like to Do you copy Well, after that again, Come on first so that then want you an online next a little is a little Confirm Now is Not I'm on the moon. The VK 2 days ago. VK 2 days. Yes. VK 2 days ago. But actually, I'm on the 2nd train in Sarabhajipa. Sorry, VK 2 days ago. From Australia to London, Sarabhajipa. So like that, if you are okay. And also, I'm here. I use for defining the class duration thing. I'm for defining the class duration thing. I'm also like morning 8 o'clock, evening 8 o'clock. Um, uh, sections are there. So you can take any for defining. So, uh, there are some, uh, I'm also taking them for taking, uh, evening, but, uh, evening, but, uh, like a fight to fight for, for defining the section. So, uh, like that. But basically here, actually, we are helping the train to improve their IQ level and also thinking about the future. So we are not that, uh, childrens are by fighting the thing. They are not going to be. But actually, we are here. We are helping the childrens how to understand the questions. They don't have by fighting or with total of them. So how they will understand the question on how they can answer it. Like that, they are teaching the childrens in class. If they steal our life, our sections are going more. Like that. Uh-huh. So, uh, the standard procedure, uh, having a doubt. So, uh, this program is, uh, complementing or, uh, are there some charges in it? Uh, I can just, uh, uh, the classes take class only 2000 to 50th class. So, uh, while you are doing the decision, you can do a, uh, the second amount of 2000 to 40 and get to human class sections. Okay. So, to have a little piece for two months, class sections for 2000 to 50th, the end of class section. Okay. So, uh, I will share the answer that is sitting on the floor. So, uh, uh, you are going to report cards. Practically, you can also do a month program. So, I will share the, uh, you need a lot of number. So, you can just do the decision. Uh, this, uh, uh, uh, okay, so, uh, thank you, thank you. I see a before fire, but you just come later, it's just not because two months time, or you need to start the class, and so do the, I'm so serious. But I got, okay. So, if you will take, if you will take for a lecture, you will take for a session, or lecture, or lecture, you will take for a few minutes. Okay. So, anyway, I will share the old details, uh, so I just go through that, and, uh, let me know. Okay. Okay. Okay. Okay.</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Soany celebrities help Heartbearing The Hello Hello you is youtube yes some little here Okay, so okay, thank you so thank you. I see it before fire. But we just come later in session that because too much time already you need to start the class and so do you have to switch today on so real but I got okay. So if you will take if you will take for a week to win so it will take for a session or a week to win you should you will take so just take it from only terminus then okay so anyway I will share the old details so I just go through that and let me know. Okay okay okay thank you have a nice day.</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>c0fec98f-91de-4349-b21d-25dc05f55eaf_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> s não é tanto hi Andy yes I'm sorry I should be a doctor I want them to be also on the beard on the one look 27 or the other I'll pick them yes I was over buying his teacher to-down graduation from that he's been qualified for the next seven days was final okay which will be on January 30th not January 30th yeah, I'm on January 30th I'm on December 30th okay, yeah, I'm on January 30th I'm happy to see you move that is full garden so if you get monthly wedding you have change on on the out is it being needed or one second I'm so once again I'll give me a second yeah, I'm so I'm being a student who the male I'm having to check it so I think I have checked it just one one second I'm just going to be your main and you have goal to keep one and then that's you yes, yes, actually I have shared long that one not a problem I was sharing two new more check members who are so important so okay, then I'm going to get a second and later we had a discussion that some of the some of the so I'm going to get a second and then then then then then then then then then then then then then then then then I'm smart this I have seen okay so first of all I've heard that when I'm a big mess in the life I'm not really a mom I'm talking to a me and you said the portrait bringing me sorry I'm you said the bringing me a me sorry sorry sorry sorry sorry sorry sorry sorry sorry sorry I'm talking to a me I'm talking to a me I'm talking to a me sorry sorry sorry sorry sorry this we more move move move move move move move極 Opening Turns out this is My Home Home Homeschool Before the A complete up to two men and a couple of three. She was given a job. Interested rain. Program. To. A. Can you. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. To. Yes. Well, Thank you. Thank you. Thank you. Thank you. Thank you. Thank you very much. Thank you so much. Thank you. Thanks for your viewing to G been an amazing experience. Thanks for your viewing to G been an amazing experience. Thank you. Yeah. Amen. Yeah. Yeah. To. Now. Go. Yeah. Are. Okay. Now we have bought. Okay. The. O. Ientsae. Yes. So. It's. enrolled now. Okay. Smoked noodles. No exactly. Not a luxury. Fried~~~ Here they are. Okay. Yes. You are the classic Shalom. You are the original form of a decent. You are the one who is making meel or you are the worst of the world. No. No. No. No. No. No. No. No. No. No. No. No. No. No. No. No. No. No. No. No. Yes. Was it a G stands? But currently they are called finals. They who are not quite popular in BED Ore series band. They take form the discs for the base for the internal instruments. Okay. This is completely up to the next class. Please do this for what we are going to do. We'll be having a teacher for the final round. Go ahead. Yes. What did you get for the final round? You are the copyboard. I'm so sorry ma. Did you have a little bit? We're going to be working on the final round. Are you serious, detective anyone is going to talk about us? Yes. In some cases, I like when we have time to talk to our parents who are with us. Have we heard them talk about us before coming home anyways? Yeah. Well, now come see itерpl is for delay and Peak from tomorrow blue time. I'm coming straight up on the 12th starting. And in December blue time if you all get the guts to go in standing for you, I try to find where I can stand right now and who help me to Get Hauptheims be? I will find so 2 months many von Haha guys I just wanted to nail these hours if you too are worrisome, I come here I am coming I am giving you something to do o nинem кажhanah Bring you two What? come on What food do these guys have? Some of them have to do food Yes sure I am not monkey my I mean up I am keeping You Native In my Canaan Eki 000 A S Onew A S A S A A A S One A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S A S S A S A S A S A S A S A S A S A S A S A S A S A S A S A A S A S A S A S A S A S A S A S A S A S A S A S A</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Un costume pose Let's send out videos The kitchen-wlesiaundani Sensei animals Shoot balls Yes I have already met her My husband called we got her She had received a good salary I will share her university number Finally She has received completely my salary of the flat first we have to complete online next time yeah yeah, I can also online next time you can attend from home with them sure, sure very smart so I would like to call the second round last year's lesson right? oh yeah so I choose her here the second round like I have been even out and I stand and I will be back with the post-censor you have to practice so I can run back to my room here or most of the time I will be back with the post-censor okay so basically here before I take them and give you a two month class for the class how the post-censor coming how they are going to answer the post-censor like that and so two months class and so that's actually going to provide the correct answer so that will also online class for the two days class of the year providing so like the Monday and the VK2 days VK2 days VK2 days so actually Monday to Sunday and VK2 days for most of the time so like that if you are okay and on social here I choose for the five minutes with the class duration thing and for the five minutes class duration then also like morning eight of the evening eight of the sections are there so I'm also thinking evening that is like a five vite five vite five five five five five five five five five four five five six six six six six six four seven six so this program is and complimenting or there are some charges in it and I feel it's a classic tape class or you do the class piece then while you are doing that at the session you can do paper, paper, mondose two-thirds of the computer piece for two-thirds of the class and you can do the class section so I will share the session and you can report and report and or process then with this there is unique image and we can fix waste and In twitch hout i Through that</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\MY WORK\openai_voice_analytics\audio.wav</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> bishop</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\MY WORK\openai_voice_analytics\audio.wav</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> boots</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> hello Hello Welcome to dishes You girls only Ladies everyone Thank you very much for meeting me to myself Thank you Permang освange Are I red에서도 I wonder informative for you yes ten minutes so you thought that it was like that it's like okay you already you are going no no no no you already I already THUYA did not dead i carry i carry skateboard so i carryš so so Pl pour And also So here I see a Defining Synthes Class Duration Then And for Defining Class Duration Then also Like Morning 8. 2 Evening 8. 1 Ah Section So there So you can take any 4 Defining So there also So I'm also them Taking Evening Backers Evening Backers Fight Fight 4 Like that But basically here Actually The thing that I Do you Do There Do And also Thinking A Busy So we All the ah Childrens Are Fighting The thing There All The Maritime Actually We are The Children's Amtus Custans We Don't Amtus Custans We Don't Amtus Custans How Like that We are Teaching The Children's Inclot This is Team Our Life As such Like Yes Okay So I'm Starting You So I'm Starting You So this program is And complementary Or Are there some charges in it? Are I Is Classic Classic Classic So We are doing that In session And You can do Paper 2 4 And 2 And Classic Okay So I will share In session And So You To Pattas To To To To To To To To To To To To To To To To To To The After You Can Just keep Convert Can So You Need to Some Basic Information about Like Like Side Side Side Side Side Side Side Side Side Side Side Side Side Side Side So You Can Convert Just keep Convert Can Just Go You Part Let You Need Part Do To You Need Part Do To To To To To We Just Convert It You Need To So Good Today I am so So You Can Can You Can You Can You You You Can You Can You Can I will share this Through That And let Me Often Often Often Often Often Often Often Often Often Often Often Often Sometimes What Sometimes</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 5- peacock of 8 . So basically here actually there is things that are doing root there, I killed avert and also thinking about the things that we all know that the childrens are by fighting the things that are out the marital. So actually there here we are helping the childrens how to understand the questions. We told a by-hunting or we told them how to remember it. So how they understand the question and how they can understand the answer like that we are teaching the childrens in class. This is teaching our life as actions as going on. Like this. Okay. Okay. So I decided to proceed you telling a faring a thousand. Also this program is incomplementary or are there some charges in it? So basically there are classes based class only two thousand rupees a class piece. So while you are doing that in session routine you can do a few more notes two thousand rupees for the end date two month class section. Okay. So further a piece for two months class. We are two months class sections for two thousand rupees. The end date class section. Okay. So I will share the session and also you are reporting practical and also two month program rolls. So I will share the you will watch the number. So you can just do the session. So this thing may hire you you will watch the session. You will be active after you can just keep going. So some because you need to fill up some basic information about that besides the data. So after the session you can share with the screen shot and also date over top and so I remember admission from IE. But tomorrow you will get the information. So you can choose any basic information you want. So you are probably recording. So you are everything you have prepared. I think for now. I will go through it. Okay. So you can just come later. Because two months time you need to start the class. So today I am so really good. Okay. So you will take you will take for a two minutes. Okay. So you need to do that. Okay. Okay. Okay. Thank you. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Because I know Hello Hello Alsoenes Yes Hello Hello Hello Hello Councillor It's And o'Connor After You said that the poor guy and the poor guy didn't expect to get lucky. Uh-huh, okay. You already know these. You are going to be. No, no, no, my children. I already wanted to. I was. Yeah, I was. I did not. Okay, okay, okay. I'm not going to see you. You see, I'm sharing. You see, there are lots of people. I'm sharing. Number twenty five 5 for you right. So, author twenty five welcome mirror lastgo, the payment giving right. We are döv Perform LGirl. Yes, hunting dead collect이스amedipp la Correct, dévelop st Everybody. Sorry.ust I be completelyNext The by the gym And don't succeed. I Sep. right. So We will see you tell a funny So this program is a complimenting or are there some charges in it? I feel that it's a classic big class of YouTube, so while you are doing that in session of time, you can do a 50M on those for the MDE Human Class section. consider a piece for the month's class. We are two months class section for 2000 pieces. MDE class section. Okay, okay. So, I will share answer version and also you are reported, practically, you can also do a month program for all so I will share the answer. You can just do the session. So, you can just do the session. So, you can just do the conversation. So, you can just do the conversation. So, because you need to feel some basic information about the like the session. You can just do aARON for an accordingly. Ah, I'm okay. Okay. Okay. So, okay. Thank you. I see a before fire. But we just completed the exercise. That because too much time or you need to start the class. So, today, I'm so real. But I am okay. So, if you will take, if you will take for you to win, if you will take for a session or only two minutes, if you will take. So, just take it from only two minutes. Okay. So, anyway, I will share the old details. So, I just go through that and let me know. Okay. Okay. Okay. Thank you. Have a nice day. Thank you. Nice.</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> now Hello hellodrumommt Lt. modern is all all have an Yes. Okay, some they continue here are actions for the how the question are coming how they are going to answer the question like that and so two months later that actually are going to prove it the correct answer. So that will not so online class for the weekly two days class of the year already. So I am going to do a weekly two days of weekly two days. So actually I am going to do some the training. So I will be sorry in the beginning and you do the you can choose from mostly to the time to do a packet of time. So like that if you are okay and on so time here I see for defining the class duration thing and for defining the class duration they are also like morning eight of the food evening eight of the action so you can take any food defined. So I will show you I am also taking a evening back just like a fight for deep fight back of actions. Like that. So basically here I see the thing that I do in root there are I kill them and also think about the thing. So we all know that ah, childrens are by fighting the thing they are out memory thing. So actually we are here we are helping the childrens how to understand the questions we don't by having or we don't have memory thing. So how they understand the question and how they can answer it. Like that, they are taking the childrens in class. This is too a section that is going like that. Okay, okay. So I decided to see you, I am having a dose. So this program is in complimenting or there are some charges in it. I kill each other with a big class or YouTube also looking to a class so ah, while you are doing that, a section of time you can do ah, a big two-tone two-tone four-dendent section. Okay, so if I have a big, two-month class section for two-tone two-tone two-dendent class section. Okay, okay. So, ah, I I was afraid, I was afraid, I was afraid, I was afraid, I was afraid, I was fire I was afraid, But the I was afraid, So after the decision, You can share with the screen show and also They go for the top and show I leave them the Admissions from I need to start. But tomorrow, We Tomorrow you look at the For some admission. Do you Show you can too And you have to see If you can You want the And Like that. Okay. Okay. So you haveouthern How are you putting your Fair? Um, I think for now. You And me, I will go through it. And Okay. Okay. Okay. Okay. Okay. Thank you sir. Thank you. I see before fire, But we just completed it. Just because Two months time, Or you need to start the class. And so, I took the day. I'm so Real. But I am okay. Okay. So, You will take, You will take Or you will Do it. You will take for a session. Or you Do it. You will take. So, just, I take it. Or you Do it. Okay. So anyway, I will share the Oldie Cancer. So I just go through that. And, I think we know Okay. Okay. Okay. Okay. Thank you. Have a nice day. Thank you. Thank you. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> into Van aquilo uh no betterking very good great uh I21 and also thank you lord it isег oh What You del So So Yeah, I'm not sure what I'm like, but I'm gonna tell you Can I tell you something? Sure Yes, Bob So I'm interested to call the second round last year, let's go Right? Oh Yeah So I choose her here The second round, like, the number you need to be Is not an I'm sure that the number you need to be The cost is only up to the right So So the third round, by the way, here, oh, I'm gonna go to the right Okay So, the second round here, before I take them, I'll give you 2 months class of actions for the trade How the cost is coming, how they are one, two, answer, That cost is like that, and so So 2 months class of actions, we are going to throw it So That will also online class of the week, two days class of the year, already So, like, the Monday, then, then The week, two days of Week, two days, yeah, so Week, two days of So, actually, Monday, two, three days of the year, so In week, two days, we can choose From most of the children's actions in our packet I found this, so like that is If you are okay, and on social here, I give A defining instance of class duration thing, and for Defending class duration, they're also like morning 8 o'clock, evening 8 o'clock Uh, actions are there, so you can take any 4 defines, so there are so So, to, um, also, children's actions, taking, uh, Evening classes, evening classes, like a fight, 2 fight, 4 define classes, actions, uh, 2 sets of, like that. But basically here, actually, they are And things are doing good there, I, 9 o'clock, and also thinking about the kids, So we are not that, uh, children's are by Fighting the things, they are not Not allowed to remember anything, But actually, they are here, we are In the children's how to understand the Costumes, we don't Aby, Fighting, or we don't To remember anything, so how they They understand the question, how they can Answer it, like that, they are Children's, in class, this is Still our life, our sections are going Like that. Uh-huh, okay, okay. So, uh, the children will see you To, uh, having a doubt. Also, uh, this, this program is, uh, And complementing, uh, Are there some charges, isn't it? I can, uh, uh, it's a class, it's Class of the year, 2000, With the class teacher. So, uh, while you are doing that, It's just a routine, you can do It's, uh, it's been On the, uh, 2000, it's For the end-day human class Okay, so, uh, To the end-day class For the end-day class For the end-day class For the end-day class So, uh, Isher, uh, Isher, uh, is So, uh, uh, You are a report card, So, after the decision, You can, uh, The share with the screenshot, and also They go for the top-up, and so I The, uh, then the admission from I, the official. But tomorrow, we, uh, tomorrow, you Look at the form admission, do you So you can do it in your Basic, basic, basic, then you want the class And then, the letter. Okay. Okay, so, you're probably Any code inside of you? How are you? Um, I think for now, You, uh, send me a little bit, Go through it, and okay, Okay. Okay. Okay, so, okay, thank you, sir, thank you. I see a big one for you, just come Later, it's just, you know, because Two months time, or you need to start the class, And so, uh, so, I treat you today, I'm so Real. But I, uh, okay. Okay. So, you do It will take, it will take for You do it for, uh, it will take for A session or you do it for You do it for, uh, so just, uh, Take it from For you do it for, uh, okay. So anyway, I insured the All the cancel, so I just go through that And, uh, let me know Okay. Okay, that's okay. Thank you. Have a nice day. Thank you, sir.</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\MY WORK\openai_voice_analytics\audio.wav</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> set up streams Download hello Welcome to the new Good afternoon This is so slow Today listen those Let's put a copy of the e-mail And just final round And i will call it from disclab because if you like, it does better according can you please so so okay so actually i want to inform you that i can use part of the first round like them and also if you can spot us i can know in upcoming level national level like them but i'm glad you did some of those but you know okay so you can give them a little bit of a little bit of regarding local port that i'm trying to give you to give you to send me a name so you said that the port can have a name that the port can have that to get okay you have already been already using you are going to not not not my to all be a name i already wanted i want to take it i did not hope okay so i'm going to show you what i want to do and share with you a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of a lot of the a lot of the and no I Shit a lot. yes now okay. so basically here before that I'm going to give you to the questions coming how they are to the questions we are so that so the one we get to we get to yes yes yes yes yes yes yes yes yes yes yes you are now continue keep I do not and with shipping basically here actually thing that I do in route there I do not and also thinking about it so we all know that the childrens are by fighting the things that are not the mariti here we are the thing that childrens how to understand the questions be told by the childrens in class and the childrens are life and so I am sorry I am sorry I am sorry I am sorry I am sorry I maybe I knew very prepared on Board and students b1 because for courses and lots of courses in class A and One the more continue ensure</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> So I need a new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new new</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Incoming c B bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum bum</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Saxon Allowing You so youちゃ ha可 You already not Yeah for the rightเล Yeah yeah Yeah Behind This Already Like the Monday The VK 2 days We get to Yes We get to this So, actually Monday to Sunday, Friday, Saturday, April, sorry We get in a new 2 days weekend too From Australia to London, South to the North Package, I found this So like that, if you are okay And also, I'm here I use for 5 minutes With the class duration thing And for the class duration There are also like morning 8 o'clock Evening 8 o'clock Uh, sections are there So you can take any 4df So, uh, there are also Uh, I'm also taking them So, taking, uh, evening Backers, evening Backers, like a fight To fight for Detail backer Fixings Uh, Tuesday Uh, Tuesday So, basically here Actually, we are helping To improve their IQ Level and also Thinking capacity So, we all know that, uh, Childrens are by fighting the things They are not numerating Actually, we are here We are helping the childrens How to understand the questions We told them by Harding or we told them How to remember it So how they learn The standard question How they can handle it Like that, they are teaching the childrens In class This 16-hour life As such, you are going more Like that Uh-huh Okay, okay So, uh, the standard question is Are you telling us? Also, uh, this program is, uh, And complementing or, uh, Are there some charges, isn't it? All right, can you turn on, uh, In class, in class, in class, 2,000, with the class Teacher, uh, So, uh, while you are doing the Decision routine, you can do Create, uh, The teacher models 2,000, because for the Ended Human Class Sentence. Okay, So, I will just put 2 months for the class And, uh, 2 months class Sentence for 2,000, with the ended Class Teacher. So, uh, are you sure? Are you sure? Are you sure? Are you sure? I am doing, uh, uh, You are Report class, Practically, you can Do a month for Grammar also Don't say, you sure, That the, uh, Watch-Up number. So, you can just do Recessions. Uh, this, It's a thing, You need a watch-up So, The Recession You need to activate. Uh, after, You can just keep Convert, you, So, it will be going So, Uh, you need to fill up Some, uh, basic Information about Okay, like, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, I, �, Toights. U, B, I, picks, bara nuevo, Ok, Copy. Copy. Copy. Copy. Copy. Copy. Copy. Copy. Good village, good excellent office has built some very good and let me know okay okay</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Please prom... Participate Have a seat, pal... Looking Want to see a movie? Queen... Maybe a girl could be brought by... Just imagine, sigma... She'syracing Where's the daughter of S啦... Call it Homeless young situations Are you kidding me? No, no... I don't know... Beheading Time to take the night off Give her another hand There she is Unauthor Foreground Yeah? Okay So actually I wanted to inform you that I've seen you before To tell you the first time I've come And also, I've been told that I've come down Upcoming the wrong national anthem But I'm glad you didn't know that possible You know? Okay So, you're getting into the mail And mail's out regarding now I'm trying to port that on certificate You do the thing Yes, it's 10 minutes Uh-huh So, you saw that the port can't have me... Uh, the port can't have certificates Uh-huh Okay You have already met no reason You are going to... No, no, no, no, no You already met me I already met you I was... Okay Okay Okay, okay So, I've been using it for a few years You know, I've been sharing it with you A lot of people have been sharing it A lot of number of people You could be able to write Okay, okay Yeah So actually, I've been told that I've come in the little national anthem And you can prove it It's a good ethnic So that I'm not going online next time Yeah? Uh-huh Yeah, I'm not going online next time You can attend some moments So, you're a small bit So, uh-uh, I'm just going to call the second round National Electronics Right? Oh Yeah So, I choose her here The second round, like, the number you need to know And, uh-uh, I'm starting to examine the demand of the post-censor layout And then, like, the number you need The most, uh-uh, the number you need to know is the number you need to know Okay, sir So, basically, you need here, uh-uh-uh Before that, I've taken the number and give you two months class for the class to how the questions are coming how they align to answer the questions like that, and so two months class that's actually a going to prove it a good answer So, that we're also online class for the weekly two days class of the year, providing So, uh-uh, like, the Monday to Monday the weekly two days of weekly two days of the year, the year, the week two days of So, actually, uh-uh, Monday to Sunday, Friday, Saturday and Sunday, Saturday, Wednesday, Saturday, Saturday and Saturday, the week two days we can choose from all three children such as you, uh-uh, packet like that is you are okay And also, so here, I see for the five minutes with the class duration thing and for the five minutes class duration, they're also like morning eight of the evening eight of the uh-uh, sections are there so you can take any four defines So, uh-uh, there also taking them to a taking a flight to a flight for a flight by the sections, uh-uh, two sections So, basically here, actually, there's things that are doing good there, I-Q-Level and also taking a bus to a new orn of the uh-uh, childrens are by-finding the things they are not going to be actually, we are helping the children how to understand the questions they are helping all the total of the number so how they understand the question how they can answer it like that, they are in class these two are life sections are going like this okay, okay so, uh-uh, the second was a little bit of a faringly dose So, uh-uh, this is-this compliment or uh-uh-uh-uh-uh are there some charges in it? Alright, so, uh-uh, it's a classic class review, two thousand rupees with a class piece, uh-uh so, uh-uh, while you are doing that, uh-uh, it's just a routine, you can do a-uh, it's a amount of two thousand rupees for two thousand rupees for two thousand rupees for two thousand rupees for the end of class section okay, okay so, uh-uh, are you sharing, uh-uh, is there any on-dotes, uh-uh, uh-uh, you are a report card practicator, no one could do one program, no one should regular words of number so, you can just do the session practice, attend me a high report, uh-uh, you can just keep going, so, um, cause, uh-uh, you need to fill up some uh-uh basic information about like, uh-uh-uh-uh-uh-uh-uh-uh, more so, uh-uh-uh-uh-uh-uh-uh, period like that, uh-uh-uh-uh-uh-uh, so, after the session is uh-uh-uh-uh-uh-uh, the share with the screenshot and also date of the top particular, uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh Round the model, we- uh-uh-uh-uh-uh-uh-uh, you look at the whole accommodation, do you saw you can't do it in your lab, did you see the secrets, did you find your one-back lab, did you find the lector? okay okay, so, you have any queries, how do you find everything you have created? um... something for now, you just uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh-uh- người okay, um... okay, okay, sorry, okay, Hanky, sorry, Hanky, I see it before Chaeok crappy systems, be 팬 chair, because a lot of time you need to start the class and so do things, huh I mean, they're so evil but I am okay it dried up so um... it would be to work if it oralion so you a... take it from only terminus, then okay, so anyway, I insure the old details are so I just go through that and uh... let me know okay, okay, okay, Hanky, have a nice day super thank you, nice</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> So many of you have been in the room. Hello. Hello. Hello. Hello. Hello. Hello. Hello. Hello. Hello. Hello. How's Dad doing all? That's all? Yeah. deteriorates. – Richard. – he fixed it. – Yeah. I'm going to play children. – I m home delivered. – I like home compressing and stuff like that. – Spot lightning fans. – They gave me handquest right back. – I'm the kind ones who are particularly good at armament. – I'm a little bit slow. – I'm actually a little bit slow. – I'm a little bit slow. – Are you able to board that one side? – Yeah. – Okay. – So actually I want to inform you that I can use my computer for the first time in the exam. – And also, if you can board this, I can know when it's upcoming, the real national exam. – That's the regulation that's possible. – Yeah. – Okay. – So you're getting the main element regarding my challenge to board card arms. – I think you can do this. – Yes, it's 10 million. – So you saw that the board card aren't meant to board cardons that to get that? – Uh-huh. – Okay. – You have already made no use. – You are going to be able to. – No, no, no. – I already made it. – I was taking it. – I did not go on. – Okay, okay. – I'm not going to show you. You can see I'm sharing a bit of a lot of non-comparing sharing. You never watch a number of things. You can do it for the right. – Okay, okay. – Yeah. – So I think I'll just let them come in and let them last. They'll let some of you get through it. They'll do it. They can make a lot of non-line next. – Yeah. – Yeah. – Yeah, they'll let some non-line next. And you can add them from home. – So, you're a smart. – So, uh, I'm just going to call the second one last. – Yeah. – Right. – Oh. – Yeah. – So, I choose her here. The second one, I can go and really think, is not. And I'm going to stand by the door and then the costumator will be up. It's right. So, the second one, I can go and look here. Or, you know, I'm going to put them around the costumator. Okay. So, the second one is here. Before I take them, I choose here, give them to my class. For the class, the costumator coming out there, one door, and the costumator like that. And so, two months class, the costumator is going to provide the class. So, that's a non-line class for people who are providing. So, I'm going to run... The VK2 data. VK2 data. Yes. VK2 data. So, I actually am going to send the trainers out of the infrastructure in VK2 data. You can choose from all the data that you are sending. So, like that, if you are okay. And also, I'm here. I choose for the five minutes with the class duration thing. And for the five minutes class, the duration thing I'm also like morning 8.2, evening 8.2. So, you can take any four designs. So, there are some, I'm also taking them to take them, evening 8.2, evening 8.2, evening 8.2, like a fight for the fight back of six months. Just like that. But basically here, actually, they are helping to improve their IQ level and also thinking about the things. So, we all know that the trainers are by fighting the things that are out of the marathon. So, actually, they are here, we are helping the trainers out to understand the questions. They told about the fighting or they told them about the marathon. So, how they are able to understand the questions and how they can handle it. And they told that they are teaching the students in class. They teach students how life affections are going like this. Okay. So, I'm starting to be thinking about having a dose. So, this program is uncomplimentary or are there some charges in it? So, I think it's a classic big class or you can do it with a class piece. So, while you are doing the decision, you can do it with your models. It's for the end date, human class section. Okay. So, I have a piece for the human class. We have two months class sections for two thousand rupees. The end date class section. Okay. So, I will share the session and also you are going to report cards. Practically, you can also do a month program. So, I will share the video. You will watch the number. So, you can just do the session. Just take me high and you will watch the group. So, the session in will be active. You can just keep going. So, you will be going. So, because you need to fill up some basic information about that like, I would say, you need to get like that. So, after the decision is, you can share with the screen shot and also date over to the end. So, I will be done by admission from I. But, tomorrow, you will get a bit more information. You can do it in your lab. It's a basic thing. You want the class section and the lecture. Okay. Okay. So, you have any queries? How are you? Everything you have said? I think for now, you have sent me a little bit of a trick. Okay. Okay. Okay. Okay. So, thank you so much. Thank you. I see a before file. Hopefully, it is just completed. It's just because two months time already, you need to start the class. So, I took the day. I'm so serious. But I am okay. So, you do it take, you do it take for a week to win. You do it take for a session or week to win. You should do it take. So, just take it from. Okay. So, anyway, I will share the old details. So, I just go through that and let me know. Okay. Okay. Okay. Thank you. Have a nice day. Thank you.</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Let me know how we deal with it How we deal with it Hello, hello Hello, hello Hello Greetings, everyone from Al-Ajcput Adresse Yes, marine المpage möchte Hi, how are you? Nice to meet you Am I clear now? My name is Ali We are at the quad continent A close this continent What are the hidden ads? Congratulations from the cement Elon Musk He has been conducting像 thisshi my soul and Xia그렇 Because of all emigres Aryavira was a trainer Yes And Actually I wonder in four minutes Electronic ground Up to the first home Except And also Because people For this机 Subcoming Now I'm going to be able to pass the book You know Okay So You're getting into the main And means Are you regarding What I'm trying to I'm certificate You're To feel it Yes It And Means Uh-huh So You saw That the For God And Get So You saw Okay You have already Men already You are No No, no, my Old man Man I already I want You are I'm taking this I did not Okay Okay, okay I'm not any sure if you I'm sharing What a lot of Not A lot of Not A lot of Not Okay Okay Yeah So, I choose I can find Upcoming National Electron I can Proceed Up So, that Roll To Next Yeah I can Roll I can I can I can I can Roll To Online Next I can I can I can I can I can I can I can I can What I can I can I can I can Roll The The So, Before the Thank you Gonna Do Like that Two months Plastic So, That Online class Two days Providing So, A Big Two days So, Actually, I'm Detailing So, I'll be in the show in Wittigin We need two days We can choose Most of the Children's So, I'm Detailing So, like that, If you are Okay. And also, Here, I choose For defining Is the class Doition And for defining Is the class Doition Then also, like Morning So, I'm So, You can take any Four Defenders. So, Roger I'm also Taking And also, Evening Like, I'll be Fighting For defining Action Like that But, Basically, here, Actually, I have been Doing Router I-Q-Level And also, Thinking I'll be Fighting The things They are Router Marry Firing Here, we are Helping The Children's How To understand The questions We thought About Fighting Or we thought Router So, how They understand The question How they can Answer Like that, The Teaching The Children's Inclot Okay, okay So, I decided to take it I'm sorry, I need a thousand So, This program is And complimentary Are there some charges, isn't it? I can tell It's a classic So, You can do Keep So, While you are doing the Recession routine, You can do Take The 2.0 For the Human Class Pension Okay, Have a Piece for And 2.0 For For the Ended Class Pension Okay, okay So, I decided I decided I decided And So, You are Report Card Practically Get Ended 1.5 For 1.5 For And 1.5 For And 1.5 For And 1.5 For And 1.5 For And 1.5 For And Every interesting $3.00 Not one Other After Recession OrHow 1.5 For And 4.0 Dropped Front For Already Open 3.10 For preserve And Part schon For And Okay Okay So Quotes How Everything You have Here I think For now You Just send me A little Go through it Okay Okay Okay Okay So Thank you Thank you I see a Before Fire For you Discomputer It's just Today I'm So Real But I Okay So It will take It will take For Recession Or It will take So Just A Decide Or It will Okay So I insure The Already Can So Just go through that And Let me Have a next Super Thank you Nice</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>f7422f49-5b42-48aa-a98c-67f1da3bda21_0_r.wav</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>oooo! hello hello hello yes, hello I'm speaking to a Aria Dian, a judge put there Aria Dian yes my name is Aria Dian and I'm on the program I'm playing a game my name is Aria Dian I'm on the program I'm on the program regarding some people that even the kind ones might be a lot of Aria Dian yes ok so actually I wanted to inform you that I see these fast phones and also the people who come and I'm going to get some passport ok so I'm getting the regarding the charity portcard certificate yes it is so you said that the portcard is ok you have already been learning learning I already I'm taking okay if you have a lot of money you can do okay yeah so actually I can have a lot of money so that you can have a lot of money you can have a lot of money so yeah so yeah so actually so I'm here the second round I'm going to do the first round and then I'm going to do the first round ok so before I do the first round I am going to have a lot of money and then I'm going to do the first round and then I am going to do the first round and then I'm going to do the first round I'll do the first round here Yes we do this But we did actually abandon the traditional things when we do this we get temperatures right down like that is that is like this we can squat and for some like morning April and so you can take any 4D so taking even back and fighting 4D back and just like that but basically here actually you have things and also thinking about the things that are fighting and here we have things that are fighting and so how they understand how they can and this is team and actions are going like that so I decided to say that I am having a doubt so this program is incomplementing or are there some charges in it? I can do a class when you are doing that you can do 3D 2D 2D and 2D and 2D and 2D and so to particular human browser on-site that watching so you can the and you can just keep going so you need to keep going so you can do a class and you can do a class and you can do a class and you can do a class and you can so are there any courses or is everything integrate for now and and it and ok Ok thank you I see before clarify I am so real but I am ok so if you will take if you will take you will take a session you will take so just take it for you ok so anyway I will share the old details so I just go through that and let me know ok ok thank you have a nice day thank you very much</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\MY WORK\openai_voice_analytics\Stored Data\audio.wav</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>C:\Users\Admin\MY WORK\openai_voice_analytics\Stored Data\audio.wav</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> doses</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>